<commit_message>
5311: cleaned up functions more, continued merging with loc
</commit_message>
<xml_diff>
--- a/5311/corrected_bad_fuzzy_match.xlsx
+++ b/5311/corrected_bad_fuzzy_match.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S154408\Documents\Assignments\Crosswalks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9874F1AC-DB4C-4E8D-A715-BFBD2F3E65E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D357B6B-CCB7-4DA9-B151-B3FB6D9D3E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="915" windowWidth="14355" windowHeight="10890"/>
+    <workbookView xWindow="-5490" yWindow="2235" windowWidth="12285" windowHeight="7770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bad_fuzzy_matches (2)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>organization_name</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Fresno Council of Governments</t>
   </si>
   <si>
-    <t>Klamath Trinity Non-Emergency Transportationâ€‹</t>
-  </si>
-  <si>
     <t>Trinity County</t>
   </si>
   <si>
@@ -155,12 +152,18 @@
   </si>
   <si>
     <t>9R02-91009</t>
+  </si>
+  <si>
+    <t>9R02-91057</t>
+  </si>
+  <si>
+    <t>Klamath Trinity Non-Emergency Transportation​</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0000#"/>
     <numFmt numFmtId="165" formatCode="000#"/>
@@ -655,7 +658,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,6 +669,8 @@
     <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -711,7 +716,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1105,11 +1117,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4">
         <v>90208</v>
@@ -1214,10 +1226,10 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1243,10 +1255,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1268,18 +1280,20 @@
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1306,85 +1320,85 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>